<commit_message>
Add purchase price parity for Goods Vehicles
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_EV_Parity.xlsx
+++ b/SuppXLS/Scen_TRA_EV_Parity.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vahid\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1E3C72-9631-45E5-BB7D-653B6ECC1B13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15895A56-314E-4EC0-8E77-3AD01762589F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="32000"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="232">
   <si>
     <t>Year</t>
   </si>
@@ -481,9 +481,6 @@
     <t>INVCOST~2050</t>
   </si>
   <si>
-    <t>~FI_T</t>
-  </si>
-  <si>
     <t>TechName</t>
   </si>
   <si>
@@ -943,7 +940,10 @@
     <t>T-CAR-BEV150*,T-TAX-BEV150*</t>
   </si>
   <si>
-    <t>T-CAR-BEV250*,T-TAX-BEV250*</t>
+    <t>T-CAR-BEV250*,T-TAX-BEV250*,T-LGT-BEV*</t>
+  </si>
+  <si>
+    <t>T-MGT-BEV*,T-HGT-BEV*</t>
   </si>
 </sst>
 </file>
@@ -2494,10 +2494,10 @@
   <dimension ref="A3:AO94"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="6" topLeftCell="H25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="6" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="A45" sqref="A45:A47"/>
+      <selection pane="bottomRight" activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2527,9 +2527,7 @@
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
-      <c r="C3" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="C3" s="18"/>
       <c r="D3" s="18"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
@@ -2549,25 +2547,25 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="E4" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>72</v>
@@ -2585,140 +2583,140 @@
         <v>76</v>
       </c>
       <c r="M4" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="N4" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="O4" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="22" t="s">
+      <c r="P4" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="Q4" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="R4" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="R4" s="23" t="s">
+      <c r="S4" s="23" t="s">
         <v>90</v>
-      </c>
-      <c r="S4" s="23" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="25" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>94</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="I5" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="J5" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="K5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="N5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="O5" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="K5" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="M5" s="26" t="s">
+      <c r="P5" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="O5" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="P5" s="27" t="s">
+      <c r="Q5" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="Q5" s="27" t="s">
+      <c r="R5" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="R5" s="26" t="s">
+      <c r="S5" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="S5" s="26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
       <c r="E6" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="K6" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="N6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="O6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="P6" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="K6" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="L6" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="M6" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="N6" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="O6" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="P6" s="30" t="s">
+      <c r="Q6" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="Q6" s="31" t="s">
+      <c r="R6" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="R6" s="30" t="s">
+      <c r="S6" s="30" t="s">
         <v>106</v>
-      </c>
-      <c r="S6" s="30" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -2741,13 +2739,13 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>122</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>123</v>
       </c>
       <c r="D8" s="17">
         <v>2019</v>
@@ -2800,13 +2798,13 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>125</v>
-      </c>
       <c r="C9" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="17">
         <v>2019</v>
@@ -2859,7 +2857,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" s="32"/>
       <c r="C10" s="32"/>
@@ -2882,13 +2880,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>126</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>127</v>
       </c>
       <c r="D11" s="17">
         <v>2019</v>
@@ -2941,13 +2939,13 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>129</v>
-      </c>
       <c r="C12" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D12" s="17">
         <v>2019</v>
@@ -3000,13 +2998,13 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>131</v>
-      </c>
       <c r="C13" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="17">
         <v>2019</v>
@@ -3059,13 +3057,13 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>133</v>
-      </c>
       <c r="C14" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" s="17">
         <v>2019</v>
@@ -3118,13 +3116,13 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="17">
         <v>2019</v>
@@ -3177,13 +3175,13 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>136</v>
-      </c>
       <c r="C16" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D16" s="17">
         <v>2019</v>
@@ -3236,13 +3234,13 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D17" s="17">
         <v>2019</v>
@@ -3295,13 +3293,13 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="17">
         <v>2019</v>
@@ -3354,13 +3352,13 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>140</v>
-      </c>
       <c r="C19" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" s="17">
         <v>2019</v>
@@ -3413,13 +3411,13 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" s="17">
         <v>2019</v>
@@ -3472,13 +3470,13 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="17">
         <v>2019</v>
@@ -3531,13 +3529,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="17" t="s">
-        <v>144</v>
-      </c>
       <c r="C22" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D22" s="17">
         <v>2019</v>
@@ -3590,13 +3588,13 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" s="17">
         <v>2019</v>
@@ -3649,13 +3647,13 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24" s="17">
         <v>2019</v>
@@ -3708,13 +3706,13 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="17">
         <v>2019</v>
@@ -3767,13 +3765,13 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="17">
         <v>2019</v>
@@ -3826,13 +3824,13 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="17">
         <v>2019</v>
@@ -3885,13 +3883,13 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="B28" s="17" t="s">
-        <v>151</v>
-      </c>
       <c r="C28" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" s="17">
         <v>2030</v>
@@ -3944,13 +3942,13 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D29" s="17">
         <v>2030</v>
@@ -4003,7 +4001,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30" s="32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
@@ -4026,13 +4024,13 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" s="17">
         <v>2019</v>
@@ -4085,13 +4083,13 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="17">
         <v>2019</v>
@@ -4144,13 +4142,13 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D33" s="17">
         <v>2019</v>
@@ -4203,13 +4201,13 @@
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" s="17">
         <v>2019</v>
@@ -4262,13 +4260,13 @@
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="17">
         <v>2019</v>
@@ -4321,13 +4319,13 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D36" s="17">
         <v>2019</v>
@@ -4380,13 +4378,13 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D37" s="17">
         <v>2019</v>
@@ -4439,13 +4437,13 @@
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="17">
         <v>2019</v>
@@ -4498,13 +4496,13 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D39" s="17">
         <v>2019</v>
@@ -4557,13 +4555,13 @@
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D40" s="17">
         <v>2019</v>
@@ -4616,13 +4614,13 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41" s="17">
         <v>2019</v>
@@ -4675,13 +4673,13 @@
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42" s="17">
         <v>2019</v>
@@ -4734,13 +4732,13 @@
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D43" s="17">
         <v>2019</v>
@@ -4793,13 +4791,13 @@
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D44" s="17">
         <v>2019</v>
@@ -4852,13 +4850,13 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D45" s="17">
         <v>2019</v>
@@ -4911,13 +4909,13 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A46" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D46" s="17">
         <v>2019</v>
@@ -4970,13 +4968,13 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A47" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="17">
         <v>2019</v>
@@ -5029,13 +5027,13 @@
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D48" s="17">
         <v>2030</v>
@@ -5088,13 +5086,13 @@
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D49" s="17">
         <v>2030</v>
@@ -5147,7 +5145,7 @@
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
@@ -5170,13 +5168,13 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D51" s="17">
         <v>2019</v>
@@ -5229,13 +5227,13 @@
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D52" s="17">
         <v>2019</v>
@@ -5288,13 +5286,13 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D53" s="17">
         <v>2019</v>
@@ -5347,13 +5345,13 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D54" s="17">
         <v>2019</v>
@@ -5406,13 +5404,13 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D55" s="17">
         <v>2030</v>
@@ -5465,7 +5463,7 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -5488,13 +5486,13 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D57" s="17">
         <v>2019</v>
@@ -5547,13 +5545,13 @@
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="17" t="s">
         <v>178</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>179</v>
       </c>
       <c r="D58" s="17">
         <v>2019</v>
@@ -5606,13 +5604,13 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D59" s="17">
         <v>2019</v>
@@ -5665,7 +5663,7 @@
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
@@ -5688,13 +5686,13 @@
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="17" t="s">
         <v>181</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>182</v>
       </c>
       <c r="D61" s="17">
         <v>2019</v>
@@ -5747,13 +5745,13 @@
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D62" s="17">
         <v>2019</v>
@@ -5806,13 +5804,13 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D63" s="17">
         <v>2019</v>
@@ -5865,13 +5863,13 @@
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D64" s="17">
         <v>2019</v>
@@ -5924,13 +5922,13 @@
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B65" s="17" t="s">
-        <v>187</v>
-      </c>
       <c r="C65" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D65" s="17">
         <v>2019</v>
@@ -5983,13 +5981,13 @@
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D66" s="17">
         <v>2030</v>
@@ -6042,13 +6040,13 @@
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D67" s="17">
         <v>2019</v>
@@ -6101,7 +6099,7 @@
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B68" s="32"/>
       <c r="C68" s="32"/>
@@ -6124,13 +6122,13 @@
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D69" s="17">
         <v>2019</v>
@@ -6183,13 +6181,13 @@
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D70" s="17">
         <v>2019</v>
@@ -6242,13 +6240,13 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D71" s="17">
         <v>2030</v>
@@ -6301,13 +6299,13 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D72" s="17">
         <v>2019</v>
@@ -6360,13 +6358,13 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D73" s="17">
         <v>2019</v>
@@ -6419,13 +6417,13 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="B74" s="17" t="s">
-        <v>196</v>
-      </c>
       <c r="C74" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D74" s="17">
         <v>2019</v>
@@ -6478,13 +6476,13 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D75" s="17">
         <v>2019</v>
@@ -6537,7 +6535,7 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="32" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B76" s="32"/>
       <c r="C76" s="32"/>
@@ -6560,13 +6558,13 @@
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D77" s="17">
         <v>2019</v>
@@ -6619,13 +6617,13 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D78" s="17">
         <v>2019</v>
@@ -6678,13 +6676,13 @@
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D79" s="17">
         <v>2030</v>
@@ -6737,13 +6735,13 @@
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D80" s="17">
         <v>2019</v>
@@ -6796,13 +6794,13 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D81" s="17">
         <v>2019</v>
@@ -6855,13 +6853,13 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D82" s="17">
         <v>2019</v>
@@ -6914,13 +6912,13 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D83" s="17">
         <v>2019</v>
@@ -6973,7 +6971,7 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B84" s="32"/>
       <c r="C84" s="32"/>
@@ -6996,13 +6994,13 @@
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A85" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D85" s="17">
         <v>2019</v>
@@ -7055,13 +7053,13 @@
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A86" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D86" s="17">
         <v>2019</v>
@@ -7114,13 +7112,13 @@
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D87" s="17">
         <v>2030</v>
@@ -7173,7 +7171,7 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A88" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B88" s="32"/>
       <c r="C88" s="32"/>
@@ -7196,13 +7194,13 @@
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B89" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="C89" s="17" t="s">
         <v>209</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>210</v>
       </c>
       <c r="D89" s="17">
         <v>2019</v>
@@ -7233,13 +7231,13 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="17" t="s">
         <v>211</v>
-      </c>
-      <c r="B90" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C90" s="17" t="s">
-        <v>212</v>
       </c>
       <c r="D90" s="17">
         <v>2019</v>
@@ -7270,13 +7268,13 @@
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A91" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="B91" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="C91" s="17" t="s">
         <v>214</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>215</v>
       </c>
       <c r="D91" s="17">
         <v>2019</v>
@@ -7307,7 +7305,7 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A92" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B92" s="32"/>
       <c r="C92" s="32"/>
@@ -7330,13 +7328,13 @@
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A93" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B93" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="C93" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="D93" s="17">
         <v>2019</v>
@@ -7367,13 +7365,13 @@
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="35" t="s">
+        <v>218</v>
+      </c>
+      <c r="B94" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C94" s="35" t="s">
         <v>219</v>
-      </c>
-      <c r="B94" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="C94" s="35" t="s">
-        <v>220</v>
       </c>
       <c r="D94" s="35">
         <v>2019</v>
@@ -7424,7 +7422,7 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
@@ -7448,7 +7446,7 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C5" s="39">
         <v>1.1379672707530148</v>
@@ -7465,7 +7463,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" s="39">
         <v>1.0965584542168487</v>
@@ -7482,7 +7480,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C7" s="39">
         <v>1.0608344672849821</v>
@@ -7499,7 +7497,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C8" s="39">
         <v>1.1160225516536051</v>
@@ -7516,7 +7514,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C9" s="39">
         <v>1.0762646400738607</v>
@@ -7533,7 +7531,7 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C10" s="44">
         <v>1.0431759912535297</v>
@@ -7550,7 +7548,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C11" s="39">
         <v>1.3735697372451618</v>
@@ -7567,7 +7565,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C12" s="39">
         <v>1.3115112514023752</v>
@@ -7584,7 +7582,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C13" s="39">
         <v>1.2556677501720317</v>
@@ -7601,7 +7599,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C14" s="39">
         <v>1.3556711000240544</v>
@@ -7618,7 +7616,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C15" s="39">
         <v>1.2947445278952026</v>
@@ -7635,7 +7633,7 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C16" s="44">
         <v>1.2411122349700614</v>
@@ -7652,7 +7650,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C17" s="39">
         <v>1.6225015859505982</v>
@@ -7669,7 +7667,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C18" s="39">
         <v>1.5386318954193954</v>
@@ -7686,7 +7684,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C19" s="39">
         <v>1.4615338246117466</v>
@@ -7703,7 +7701,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C20" s="39">
         <v>1.6087314002771664</v>
@@ -7720,7 +7718,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C21" s="39">
         <v>1.5254207827911861</v>
@@ -7737,7 +7735,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C22" s="46">
         <v>1.4500804551190218</v>
@@ -7754,7 +7752,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -7768,7 +7766,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7779,7 +7777,7 @@
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="34" width="10.6640625" customWidth="1"/>
     <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
@@ -7847,7 +7845,7 @@
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>71</v>
@@ -7865,7 +7863,7 @@
         <v>20.290144783549959</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>71</v>
@@ -7884,7 +7882,7 @@
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>71</v>
@@ -7905,7 +7903,7 @@
       </c>
       <c r="G9" s="45"/>
       <c r="H9" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I9" s="45" t="s">
         <v>71</v>
@@ -7926,7 +7924,7 @@
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>71</v>
@@ -7948,7 +7946,7 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>71</v>
@@ -7970,7 +7968,7 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>71</v>
@@ -7992,7 +7990,7 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>71</v>
@@ -8014,7 +8012,7 @@
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I14" s="45" t="s">
         <v>71</v>
@@ -8035,7 +8033,7 @@
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>71</v>
@@ -8051,12 +8049,12 @@
         <v>2018</v>
       </c>
       <c r="F16" s="47">
-        <f>Original!I27</f>
-        <v>30.275999999999996</v>
+        <f>Original!H27</f>
+        <v>32.970999999999997</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>71</v>
@@ -8077,7 +8075,7 @@
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>71</v>
@@ -8098,7 +8096,7 @@
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>71</v>
@@ -8119,7 +8117,7 @@
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I19" s="45" t="s">
         <v>71</v>
@@ -8140,17 +8138,108 @@
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="14">
+        <v>2018</v>
+      </c>
+      <c r="F21" s="47">
+        <f>Original!H83</f>
+        <v>345.67</v>
+      </c>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D22" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="14">
+        <v>2025</v>
+      </c>
+      <c r="F22" s="47">
+        <f>Original!I77*'TIMES-DK'!D22</f>
+        <v>125.7421367146719</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="14">
+        <v>2030</v>
+      </c>
+      <c r="F23" s="47">
+        <f>Original!J77*'TIMES-DK'!E22</f>
+        <v>122.40478175109922</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H24" s="17"/>
+      <c r="D24" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" s="45">
+        <v>2035</v>
+      </c>
+      <c r="F24" s="47">
+        <f>Original!K77</f>
+        <v>100.95</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="16">
+        <v>2050</v>
+      </c>
+      <c r="F25" s="49">
+        <f>F24</f>
+        <v>100.95</v>
+      </c>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H26" s="17"/>

</xml_diff>

<commit_message>
Modify Purchase Price Parity for EVs
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_EV_Parity.xlsx
+++ b/SuppXLS/Scen_TRA_EV_Parity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15895A56-314E-4EC0-8E77-3AD01762589F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAEECA-4624-41F8-ACF8-53690FB16BDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7766,7 +7766,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7859,8 +7859,8 @@
         <v>2025</v>
       </c>
       <c r="F7" s="47">
-        <f>Original!I11</f>
-        <v>20.290144783549959</v>
+        <f>F6*0.9</f>
+        <v>29.673899999999996</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>228</v>
@@ -7877,8 +7877,8 @@
         <v>2030</v>
       </c>
       <c r="F8" s="47">
-        <f>F7</f>
-        <v>20.290144783549959</v>
+        <f>0.5*(F7+F9)</f>
+        <v>24.982022391774976</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
@@ -7898,7 +7898,7 @@
         <v>2035</v>
       </c>
       <c r="F9" s="48">
-        <f>F8</f>
+        <f>F10</f>
         <v>20.290144783549959</v>
       </c>
       <c r="G9" s="45"/>
@@ -7919,7 +7919,7 @@
         <v>2050</v>
       </c>
       <c r="F10" s="49">
-        <f>F9</f>
+        <f>Original!I11</f>
         <v>20.290144783549959</v>
       </c>
       <c r="G10" s="16"/>
@@ -7963,8 +7963,8 @@
         <v>2025</v>
       </c>
       <c r="F12" s="47">
-        <f>Original!I12*'TIMES-DK'!D16</f>
-        <v>24.672343382240893</v>
+        <f>F11*0.9</f>
+        <v>29.673899999999996</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
@@ -7985,8 +7985,8 @@
         <v>2030</v>
       </c>
       <c r="F13" s="47">
-        <f>Original!I12</f>
-        <v>21.831587082756254</v>
+        <f>0.5*(F12+F14)</f>
+        <v>25.752743541378123</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
@@ -8007,7 +8007,7 @@
         <v>2035</v>
       </c>
       <c r="F14" s="47">
-        <f>F13</f>
+        <f>Original!I12</f>
         <v>21.831587082756254</v>
       </c>
       <c r="G14" s="14"/>
@@ -8028,7 +8028,7 @@
         <v>2050</v>
       </c>
       <c r="F15" s="49">
-        <f>F14</f>
+        <f>Original!I12</f>
         <v>21.831587082756254</v>
       </c>
       <c r="G15" s="16"/>
@@ -8070,8 +8070,8 @@
         <v>2025</v>
       </c>
       <c r="F17" s="47">
-        <f>Original!H12*'TIMES-DK'!D22</f>
-        <v>27.920569646645671</v>
+        <f>F16*0.9</f>
+        <v>29.673899999999996</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
@@ -8091,8 +8091,8 @@
         <v>2030</v>
       </c>
       <c r="F18" s="47">
-        <f>AVERAGE(F17,F19)</f>
-        <v>24.876078364700962</v>
+        <f>F17*0.9</f>
+        <v>26.706509999999998</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="s">
@@ -8112,8 +8112,8 @@
         <v>2035</v>
       </c>
       <c r="F19" s="47">
-        <f>Original!K12</f>
-        <v>21.831587082756254</v>
+        <f>F18*0.85</f>
+        <v>22.700533499999999</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14" t="s">
@@ -8133,7 +8133,7 @@
         <v>2050</v>
       </c>
       <c r="F20" s="49">
-        <f>F19</f>
+        <f>F15</f>
         <v>21.831587082756254</v>
       </c>
       <c r="G20" s="16"/>
@@ -8171,8 +8171,8 @@
         <v>2025</v>
       </c>
       <c r="F22" s="47">
-        <f>Original!I77*'TIMES-DK'!D22</f>
-        <v>125.7421367146719</v>
+        <f>F21*0.9</f>
+        <v>311.10300000000001</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14" t="s">
@@ -8190,8 +8190,8 @@
         <v>2030</v>
       </c>
       <c r="F23" s="47">
-        <f>Original!J77*'TIMES-DK'!E22</f>
-        <v>122.40478175109922</v>
+        <f>F22*0.8</f>
+        <v>248.88240000000002</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14" t="s">
@@ -8209,8 +8209,8 @@
         <v>2035</v>
       </c>
       <c r="F24" s="47">
-        <f>Original!K77</f>
-        <v>100.95</v>
+        <f>F23*0.8</f>
+        <v>199.10592000000003</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14" t="s">
@@ -8230,7 +8230,7 @@
         <v>2050</v>
       </c>
       <c r="F25" s="49">
-        <f>F24</f>
+        <f>Original!K77</f>
         <v>100.95</v>
       </c>
       <c r="G25" s="16"/>

</xml_diff>

<commit_message>
TRA: Rename TRAHYD to TRAH2; closes #121
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_EV_Parity.xlsx
+++ b/SuppXLS/Scen_TRA_EV_Parity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAEECA-4624-41F8-ACF8-53690FB16BDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7AC02D6-B905-4EF9-ABC8-70E2120EDC51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -700,9 +700,6 @@
     <t>T-CAR-ICE_HYD21</t>
   </si>
   <si>
-    <t>TRAHYD</t>
-  </si>
-  <si>
     <t>T-CAR-FCV_HYD21</t>
   </si>
   <si>
@@ -944,6 +941,9 @@
   </si>
   <si>
     <t>T-MGT-BEV*,T-HGT-BEV*</t>
+  </si>
+  <si>
+    <t>TRAH2</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1352,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>22860</xdr:colOff>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1726,44 +1726,44 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="7"/>
+    <col min="29" max="29" width="5.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="str" cm="1">
         <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
         <v>IE</v>
@@ -1877,12 +1877,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>41</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>44</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>45</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>46</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>47</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>48</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>49</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>50</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>51</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>53</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>54</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>55</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>56</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>57</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>58</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>59</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>60</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>61</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>62</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>63</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>64</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>65</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>66</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>67</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>68</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>69</v>
       </c>
@@ -2473,7 +2473,7 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>22860</xdr:colOff>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -2494,37 +2494,37 @@
   <dimension ref="A3:AO94"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="7" ySplit="6" topLeftCell="H60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="6" topLeftCell="H71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="H75" sqref="H75"/>
+      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
     <col min="8" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="32" width="10.6640625" customWidth="1"/>
-    <col min="33" max="33" width="10.6640625" style="7" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="32" width="10.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" style="7" customWidth="1"/>
+    <col min="34" max="34" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18"/>
@@ -2545,7 +2545,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>77</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>91</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="28" t="s">
         <v>101</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>107</v>
       </c>
@@ -2737,7 +2737,7 @@
       <c r="R7" s="32"/>
       <c r="S7" s="32"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>120</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>123</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>108</v>
       </c>
@@ -2878,7 +2878,7 @@
       <c r="R10" s="32"/>
       <c r="S10" s="32"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>125</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>127</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>129</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>131</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>133</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>134</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>136</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>137</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>138</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>140</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>141</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>142</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>144</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>145</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>146</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>147</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>148</v>
       </c>
@@ -3881,12 +3881,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>149</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>126</v>
@@ -3940,12 +3940,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>126</v>
@@ -3999,7 +3999,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>109</v>
       </c>
@@ -4022,9 +4022,9 @@
       <c r="R30" s="32"/>
       <c r="S30" s="32"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B31" s="17" t="s">
         <v>121</v>
@@ -4081,9 +4081,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="17" t="s">
         <v>128</v>
@@ -4140,9 +4140,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" s="17" t="s">
         <v>130</v>
@@ -4199,9 +4199,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B34" s="17" t="s">
         <v>132</v>
@@ -4258,9 +4258,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>121</v>
@@ -4317,9 +4317,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B36" s="17" t="s">
         <v>135</v>
@@ -4376,9 +4376,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B37" s="17" t="s">
         <v>121</v>
@@ -4435,9 +4435,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B38" s="17" t="s">
         <v>128</v>
@@ -4494,9 +4494,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B39" s="17" t="s">
         <v>139</v>
@@ -4553,9 +4553,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B40" s="17" t="s">
         <v>139</v>
@@ -4612,9 +4612,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B41" s="17" t="s">
         <v>139</v>
@@ -4671,9 +4671,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="17" t="s">
         <v>143</v>
@@ -4730,9 +4730,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B43" s="17" t="s">
         <v>143</v>
@@ -4789,9 +4789,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B44" s="17" t="s">
         <v>143</v>
@@ -4848,9 +4848,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B45" s="17" t="s">
         <v>124</v>
@@ -4907,9 +4907,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B46" s="17" t="s">
         <v>124</v>
@@ -4966,9 +4966,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>124</v>
@@ -5025,12 +5025,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>126</v>
@@ -5084,12 +5084,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>126</v>
@@ -5143,7 +5143,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>110</v>
       </c>
@@ -5166,9 +5166,9 @@
       <c r="R50" s="32"/>
       <c r="S50" s="32"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B51" s="17" t="s">
         <v>128</v>
@@ -5225,9 +5225,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>135</v>
@@ -5284,9 +5284,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" s="17" t="s">
         <v>132</v>
@@ -5343,9 +5343,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B54" s="17" t="s">
         <v>124</v>
@@ -5402,12 +5402,12 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>126</v>
@@ -5461,7 +5461,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>111</v>
       </c>
@@ -5484,9 +5484,9 @@
       <c r="R56" s="32"/>
       <c r="S56" s="32"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B57" s="17" t="s">
         <v>124</v>
@@ -5543,15 +5543,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B58" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D58" s="17">
         <v>2019</v>
@@ -5602,15 +5602,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B59" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D59" s="17">
         <v>2019</v>
@@ -5661,7 +5661,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="32" t="s">
         <v>112</v>
       </c>
@@ -5684,15 +5684,15 @@
       <c r="R60" s="32"/>
       <c r="S60" s="32"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B61" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D61" s="17">
         <v>2019</v>
@@ -5743,15 +5743,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B62" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D62" s="17">
         <v>2019</v>
@@ -5802,15 +5802,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>143</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D63" s="17">
         <v>2019</v>
@@ -5861,15 +5861,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B64" s="17" t="s">
         <v>132</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D64" s="17">
         <v>2019</v>
@@ -5920,15 +5920,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="B65" s="17" t="s">
-        <v>186</v>
-      </c>
       <c r="C65" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D65" s="17">
         <v>2019</v>
@@ -5979,15 +5979,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D66" s="17">
         <v>2030</v>
@@ -6038,15 +6038,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B67" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D67" s="17">
         <v>2019</v>
@@ -6097,7 +6097,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="32" t="s">
         <v>113</v>
       </c>
@@ -6120,15 +6120,15 @@
       <c r="R68" s="32"/>
       <c r="S68" s="32"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D69" s="17">
         <v>2019</v>
@@ -6179,15 +6179,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B70" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D70" s="17">
         <v>2019</v>
@@ -6238,15 +6238,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D71" s="17">
         <v>2030</v>
@@ -6297,15 +6297,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>132</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D72" s="17">
         <v>2019</v>
@@ -6356,15 +6356,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B73" s="17" t="s">
         <v>132</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D73" s="17">
         <v>2019</v>
@@ -6415,15 +6415,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B74" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B74" s="17" t="s">
-        <v>195</v>
-      </c>
       <c r="C74" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D74" s="17">
         <v>2019</v>
@@ -6474,15 +6474,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B75" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D75" s="17">
         <v>2019</v>
@@ -6533,7 +6533,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76" s="32" t="s">
         <v>114</v>
       </c>
@@ -6556,15 +6556,15 @@
       <c r="R76" s="32"/>
       <c r="S76" s="32"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B77" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D77" s="17">
         <v>2019</v>
@@ -6615,15 +6615,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B78" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D78" s="17">
         <v>2019</v>
@@ -6674,15 +6674,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D79" s="17">
         <v>2030</v>
@@ -6733,15 +6733,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B80" s="17" t="s">
         <v>132</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D80" s="17">
         <v>2019</v>
@@ -6792,15 +6792,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B81" s="17" t="s">
         <v>132</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D81" s="17">
         <v>2019</v>
@@ -6851,15 +6851,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D82" s="17">
         <v>2019</v>
@@ -6910,15 +6910,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B83" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D83" s="17">
         <v>2019</v>
@@ -6969,7 +6969,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84" s="32" t="s">
         <v>115</v>
       </c>
@@ -6992,15 +6992,15 @@
       <c r="R84" s="32"/>
       <c r="S84" s="32"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B85" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D85" s="17">
         <v>2019</v>
@@ -7051,15 +7051,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B86" s="17" t="s">
         <v>124</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D86" s="17">
         <v>2019</v>
@@ -7110,15 +7110,15 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="17">
         <v>2030</v>
@@ -7169,7 +7169,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="32" t="s">
         <v>116</v>
       </c>
@@ -7192,15 +7192,15 @@
       <c r="R88" s="32"/>
       <c r="S88" s="32"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B89" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="C89" s="17" t="s">
         <v>208</v>
-      </c>
-      <c r="C89" s="17" t="s">
-        <v>209</v>
       </c>
       <c r="D89" s="17">
         <v>2019</v>
@@ -7229,15 +7229,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B90" s="17" t="s">
         <v>128</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D90" s="17">
         <v>2019</v>
@@ -7266,15 +7266,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B91" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="C91" s="17" t="s">
         <v>213</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>214</v>
       </c>
       <c r="D91" s="17">
         <v>2019</v>
@@ -7303,7 +7303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" s="32" t="s">
         <v>117</v>
       </c>
@@ -7326,15 +7326,15 @@
       <c r="R92" s="32"/>
       <c r="S92" s="32"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="B93" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="C93" s="17" t="s">
         <v>216</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>217</v>
       </c>
       <c r="D93" s="17">
         <v>2019</v>
@@ -7363,15 +7363,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="B94" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="C94" s="35" t="s">
         <v>218</v>
-      </c>
-      <c r="B94" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="C94" s="35" t="s">
-        <v>219</v>
       </c>
       <c r="D94" s="35">
         <v>2019</v>
@@ -7411,25 +7411,25 @@
   <dimension ref="B3:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:F16"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
       <c r="F3" s="38"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="41"/>
       <c r="C4" s="42">
         <v>2020</v>
@@ -7444,9 +7444,9 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="39">
         <v>1.1379672707530148</v>
@@ -7461,9 +7461,9 @@
         <v>1.0152168550200416</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="39">
         <v>1.0965584542168487</v>
@@ -7478,9 +7478,9 @@
         <v>0.99950497151451945</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="39">
         <v>1.0608344672849821</v>
@@ -7495,9 +7495,9 @@
         <v>0.97549719420789438</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C8" s="39">
         <v>1.1160225516536051</v>
@@ -7512,9 +7512,9 @@
         <v>0.99346955426624672</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C9" s="39">
         <v>1.0762646400738607</v>
@@ -7529,9 +7529,9 @@
         <v>0.98031421316297396</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="44">
         <v>1.0431759912535297</v>
@@ -7546,9 +7546,9 @@
         <v>0.95900971346193919</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C11" s="39">
         <v>1.3735697372451618</v>
@@ -7563,9 +7563,9 @@
         <v>1.1365210128187446</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C12" s="39">
         <v>1.3115112514023752</v>
@@ -7580,9 +7580,9 @@
         <v>1.1154653616406478</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C13" s="39">
         <v>1.2556677501720317</v>
@@ -7597,9 +7597,9 @@
         <v>1.0762352842237271</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C14" s="39">
         <v>1.3556711000240544</v>
@@ -7614,9 +7614,9 @@
         <v>1.1144919805829321</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C15" s="39">
         <v>1.2947445278952026</v>
@@ -7631,9 +7631,9 @@
         <v>1.0959457863813349</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C16" s="44">
         <v>1.2411122349700614</v>
@@ -7648,9 +7648,9 @@
         <v>1.0594421546674553</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C17" s="39">
         <v>1.6225015859505982</v>
@@ -7665,9 +7665,9 @@
         <v>1.2604972977468007</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" s="39">
         <v>1.5386318954193954</v>
@@ -7682,9 +7682,9 @@
         <v>1.2339835364748879</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C19" s="39">
         <v>1.4615338246117466</v>
@@ -7699,9 +7699,9 @@
         <v>1.1791965278222314</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C20" s="39">
         <v>1.6087314002771664</v>
@@ -7716,9 +7716,9 @@
         <v>1.2348089941373108</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="37" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C21" s="39">
         <v>1.5254207827911861</v>
@@ -7733,9 +7733,9 @@
         <v>1.2108943927694757</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C22" s="46">
         <v>1.4500804551190218</v>
@@ -7750,9 +7750,9 @@
         <v>1.1592783829087885</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="43" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -7765,34 +7765,34 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="34" width="10.7109375" customWidth="1"/>
+    <col min="35" max="35" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -7804,7 +7804,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
@@ -7830,7 +7830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14" t="s">
@@ -7845,13 +7845,13 @@
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D7" s="14" t="s">
         <v>70</v>
       </c>
@@ -7863,13 +7863,13 @@
         <v>29.673899999999996</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I7" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D8" s="14" t="s">
         <v>70</v>
       </c>
@@ -7882,13 +7882,13 @@
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45" t="s">
@@ -7903,13 +7903,13 @@
       </c>
       <c r="G9" s="45"/>
       <c r="H9" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I9" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
       <c r="D10" s="16" t="s">
@@ -7924,13 +7924,13 @@
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -7946,13 +7946,13 @@
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -7968,13 +7968,13 @@
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -7990,13 +7990,13 @@
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -8012,13 +8012,13 @@
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I14" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
@@ -8033,13 +8033,13 @@
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
@@ -8054,13 +8054,13 @@
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14" t="s">
@@ -8075,13 +8075,13 @@
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14" t="s">
@@ -8096,13 +8096,13 @@
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="45" t="s">
@@ -8117,13 +8117,13 @@
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I19" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16" t="s">
@@ -8138,13 +8138,13 @@
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="16" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D21" s="14" t="s">
         <v>70</v>
       </c>
@@ -8157,13 +8157,13 @@
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D22" s="14" t="s">
         <v>70</v>
       </c>
@@ -8176,13 +8176,13 @@
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D23" s="14" t="s">
         <v>70</v>
       </c>
@@ -8195,13 +8195,13 @@
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D24" s="45" t="s">
         <v>70</v>
       </c>
@@ -8214,13 +8214,13 @@
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I24" s="45" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
       <c r="D25" s="16" t="s">
@@ -8235,13 +8235,13 @@
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26" s="17"/>
     </row>
   </sheetData>

</xml_diff>